<commit_message>
chore: uppload (antimony fix)
</commit_message>
<xml_diff>
--- a/LME/parser_beta_2.0/data/antimony.xlsx
+++ b/LME/parser_beta_2.0/data/antimony.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="490">
   <si>
     <t>Date</t>
   </si>
@@ -1478,6 +1478,12 @@
   </si>
   <si>
     <t>2026-02-13</t>
+  </si>
+  <si>
+    <t>148008</t>
+  </si>
+  <si>
+    <t>168000</t>
   </si>
 </sst>
 </file>
@@ -8570,46 +8576,46 @@
     </row>
     <row r="483" spans="1:3">
       <c r="A483" s="1">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B483" t="s">
         <v>484</v>
       </c>
-      <c r="C483">
-        <v>21454.4</v>
+      <c r="C483" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="484" spans="1:3">
       <c r="A484" s="1">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B484" t="s">
         <v>485</v>
       </c>
-      <c r="C484">
-        <v>21445.43</v>
+      <c r="C484" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="485" spans="1:3">
       <c r="A485" s="1">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B485" t="s">
         <v>486</v>
       </c>
-      <c r="C485">
-        <v>21478.58</v>
+      <c r="C485" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="486" spans="1:3">
       <c r="A486" s="1">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B486" t="s">
         <v>487</v>
       </c>
-      <c r="C486">
-        <v>21475.48</v>
+      <c r="C486" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>